<commit_message>
Add latest developments in OECD membership
</commit_message>
<xml_diff>
--- a/Codes_Crosswalk.xlsx
+++ b/Codes_Crosswalk.xlsx
@@ -10160,7 +10160,7 @@
         <v>238</v>
       </c>
       <c r="U95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V95" t="n">
         <v>0</v>
@@ -34612,9 +34612,7 @@
       <c r="R446"/>
       <c r="S446"/>
       <c r="T446"/>
-      <c r="U446" t="n">
-        <v>0</v>
-      </c>
+      <c r="U446"/>
       <c r="V446" t="n">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Add spelling for Vietnam
</commit_message>
<xml_diff>
--- a/Codes_Crosswalk.xlsx
+++ b/Codes_Crosswalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc9855b04cee0f8c/Software/Codes-Crosswalk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{38F06027-B67A-4AF1-B3C5-C121FE7A1078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A01000D7-68B1-4400-8220-4E28032CBB48}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{38F06027-B67A-4AF1-B3C5-C121FE7A1078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7D1F285-F7EE-4B47-953B-9BE7EA6B099D}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Codes" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4871" uniqueCount="1100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4881" uniqueCount="1101">
   <si>
     <t>ISO3166.3</t>
   </si>
@@ -3322,6 +3322,9 @@
   </si>
   <si>
     <t>Federal Republic Of Germany</t>
+  </si>
+  <si>
+    <t>Democratic Republic Of Vietnam</t>
   </si>
 </sst>
 </file>
@@ -3382,6 +3385,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3663,7 +3670,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y506"/>
+  <dimension ref="A1:Y507"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -36007,7 +36014,7 @@
         <v>994</v>
       </c>
       <c r="C488" t="s">
-        <v>996</v>
+        <v>1100</v>
       </c>
       <c r="D488" t="s">
         <v>37</v>
@@ -36075,7 +36082,7 @@
         <v>994</v>
       </c>
       <c r="C489" t="s">
-        <v>1098</v>
+        <v>996</v>
       </c>
       <c r="D489" t="s">
         <v>37</v>
@@ -36143,7 +36150,7 @@
         <v>994</v>
       </c>
       <c r="C490" t="s">
-        <v>1050</v>
+        <v>1098</v>
       </c>
       <c r="D490" t="s">
         <v>37</v>
@@ -36211,7 +36218,7 @@
         <v>994</v>
       </c>
       <c r="C491" t="s">
-        <v>1069</v>
+        <v>1050</v>
       </c>
       <c r="D491" t="s">
         <v>37</v>
@@ -36273,28 +36280,28 @@
     </row>
     <row r="492" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A492" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="B492" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="C492" t="s">
-        <v>999</v>
+        <v>1069</v>
       </c>
       <c r="D492" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="E492">
-        <v>9</v>
+        <v>142</v>
       </c>
       <c r="F492" t="s">
-        <v>345</v>
+        <v>198</v>
       </c>
       <c r="G492">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="J492">
-        <v>548</v>
+        <v>704</v>
       </c>
       <c r="K492">
         <v>0</v>
@@ -36303,13 +36310,13 @@
         <v>0</v>
       </c>
       <c r="M492">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N492" t="s">
         <v>31</v>
       </c>
       <c r="O492" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="P492" t="s">
         <v>52</v>
@@ -36318,10 +36325,10 @@
         <v>99</v>
       </c>
       <c r="R492" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="T492">
-        <v>846</v>
+        <v>582</v>
       </c>
       <c r="U492">
         <v>0</v>
@@ -36333,21 +36340,21 @@
         <v>0</v>
       </c>
       <c r="X492">
-        <v>167</v>
+        <v>107.833333</v>
       </c>
       <c r="Y492">
-        <v>-16</v>
+        <v>16.166667</v>
       </c>
     </row>
     <row r="493" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A493" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="B493" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="C493" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="D493" t="s">
         <v>97</v>
@@ -36356,13 +36363,13 @@
         <v>9</v>
       </c>
       <c r="F493" t="s">
-        <v>98</v>
+        <v>345</v>
       </c>
       <c r="G493">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="J493">
-        <v>876</v>
+        <v>548</v>
       </c>
       <c r="K493">
         <v>0</v>
@@ -36371,11 +36378,26 @@
         <v>0</v>
       </c>
       <c r="M493">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N493" t="s">
         <v>31</v>
       </c>
+      <c r="O493" t="s">
+        <v>51</v>
+      </c>
+      <c r="P493" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q493" t="s">
+        <v>99</v>
+      </c>
+      <c r="R493" t="s">
+        <v>42</v>
+      </c>
+      <c r="T493">
+        <v>846</v>
+      </c>
       <c r="U493">
         <v>0</v>
       </c>
@@ -36386,10 +36408,10 @@
         <v>0</v>
       </c>
       <c r="X493">
-        <v>-176.2</v>
+        <v>167</v>
       </c>
       <c r="Y493">
-        <v>-13.3</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="494" spans="1:25" x14ac:dyDescent="0.35">
@@ -36400,7 +36422,7 @@
         <v>1001</v>
       </c>
       <c r="C494" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D494" t="s">
         <v>97</v>
@@ -36453,7 +36475,7 @@
         <v>1001</v>
       </c>
       <c r="C495" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="D495" t="s">
         <v>97</v>
@@ -36506,7 +36528,7 @@
         <v>1001</v>
       </c>
       <c r="C496" t="s">
-        <v>1087</v>
+        <v>1004</v>
       </c>
       <c r="D496" t="s">
         <v>97</v>
@@ -36553,13 +36575,13 @@
     </row>
     <row r="497" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A497" t="s">
-        <v>1005</v>
+        <v>1000</v>
       </c>
       <c r="B497" t="s">
-        <v>1006</v>
+        <v>1001</v>
       </c>
       <c r="C497" t="s">
-        <v>1007</v>
+        <v>1087</v>
       </c>
       <c r="D497" t="s">
         <v>97</v>
@@ -36574,7 +36596,7 @@
         <v>61</v>
       </c>
       <c r="J497">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="K497">
         <v>0</v>
@@ -36583,26 +36605,11 @@
         <v>0</v>
       </c>
       <c r="M497">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N497" t="s">
         <v>31</v>
       </c>
-      <c r="O497" t="s">
-        <v>68</v>
-      </c>
-      <c r="P497" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q497" t="s">
-        <v>99</v>
-      </c>
-      <c r="R497" t="s">
-        <v>42</v>
-      </c>
-      <c r="T497">
-        <v>862</v>
-      </c>
       <c r="U497">
         <v>0</v>
       </c>
@@ -36613,63 +36620,63 @@
         <v>0</v>
       </c>
       <c r="X497">
-        <v>-172.13333299999999</v>
+        <v>-176.2</v>
       </c>
       <c r="Y497">
-        <v>-13.8</v>
+        <v>-13.3</v>
       </c>
     </row>
     <row r="498" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A498" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="B498" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="C498" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="D498" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="E498">
-        <v>142</v>
+        <v>9</v>
       </c>
       <c r="F498" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="G498">
-        <v>145</v>
+        <v>61</v>
       </c>
       <c r="J498">
-        <v>887</v>
+        <v>882</v>
       </c>
       <c r="K498">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L498">
         <v>0</v>
       </c>
       <c r="M498">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N498" t="s">
         <v>31</v>
       </c>
       <c r="O498" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="P498" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="Q498" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="R498" t="s">
         <v>42</v>
       </c>
       <c r="T498">
-        <v>474</v>
+        <v>862</v>
       </c>
       <c r="U498">
         <v>0</v>
@@ -36678,13 +36685,13 @@
         <v>0</v>
       </c>
       <c r="W498">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X498">
-        <v>47.5</v>
+        <v>-172.13333299999999</v>
       </c>
       <c r="Y498">
-        <v>15.5</v>
+        <v>-13.8</v>
       </c>
     </row>
     <row r="499" spans="1:25" x14ac:dyDescent="0.35">
@@ -36695,7 +36702,7 @@
         <v>1009</v>
       </c>
       <c r="C499" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="D499" t="s">
         <v>37</v>
@@ -36763,7 +36770,7 @@
         <v>1009</v>
       </c>
       <c r="C500" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D500" t="s">
         <v>37</v>
@@ -36831,7 +36838,7 @@
         <v>1009</v>
       </c>
       <c r="C501" t="s">
-        <v>1044</v>
+        <v>1012</v>
       </c>
       <c r="D501" t="s">
         <v>37</v>
@@ -36899,7 +36906,7 @@
         <v>1009</v>
       </c>
       <c r="C502" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="D502" t="s">
         <v>37</v>
@@ -36961,37 +36968,31 @@
     </row>
     <row r="503" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A503" t="s">
-        <v>1013</v>
+        <v>1008</v>
       </c>
       <c r="B503" t="s">
-        <v>1014</v>
+        <v>1009</v>
       </c>
       <c r="C503" t="s">
-        <v>1015</v>
+        <v>1047</v>
       </c>
       <c r="D503" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="E503">
-        <v>2</v>
+        <v>142</v>
       </c>
       <c r="F503" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="G503">
-        <v>202</v>
-      </c>
-      <c r="H503" t="s">
-        <v>209</v>
-      </c>
-      <c r="I503">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="J503">
-        <v>710</v>
+        <v>887</v>
       </c>
       <c r="K503">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L503">
         <v>0</v>
@@ -37003,19 +37004,19 @@
         <v>31</v>
       </c>
       <c r="O503" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="P503" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="Q503" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="R503" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="T503">
-        <v>199</v>
+        <v>474</v>
       </c>
       <c r="U503">
         <v>0</v>
@@ -37024,24 +37025,24 @@
         <v>0</v>
       </c>
       <c r="W503">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X503">
-        <v>23.120999999999999</v>
+        <v>47.5</v>
       </c>
       <c r="Y503">
-        <v>-30.558</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="504" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A504" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B504" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="C504" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="D504" t="s">
         <v>48</v>
@@ -37056,19 +37057,19 @@
         <v>202</v>
       </c>
       <c r="H504" t="s">
-        <v>107</v>
+        <v>209</v>
       </c>
       <c r="I504">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J504">
-        <v>894</v>
+        <v>710</v>
       </c>
       <c r="K504">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L504">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M504">
         <v>0</v>
@@ -37077,22 +37078,19 @@
         <v>31</v>
       </c>
       <c r="O504" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="P504" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="Q504" t="s">
         <v>49</v>
       </c>
       <c r="R504" t="s">
-        <v>42</v>
-      </c>
-      <c r="S504" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="T504">
-        <v>754</v>
+        <v>199</v>
       </c>
       <c r="U504">
         <v>0</v>
@@ -37104,21 +37102,21 @@
         <v>0</v>
       </c>
       <c r="X504">
-        <v>28.5</v>
+        <v>23.120999999999999</v>
       </c>
       <c r="Y504">
-        <v>-14.33333</v>
+        <v>-30.558</v>
       </c>
     </row>
     <row r="505" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A505" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B505" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="C505" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="D505" t="s">
         <v>48</v>
@@ -37139,10 +37137,10 @@
         <v>14</v>
       </c>
       <c r="J505">
-        <v>716</v>
+        <v>894</v>
       </c>
       <c r="K505">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L505">
         <v>1</v>
@@ -37157,80 +37155,157 @@
         <v>51</v>
       </c>
       <c r="P505" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="Q505" t="s">
         <v>49</v>
       </c>
       <c r="R505" t="s">
+        <v>42</v>
+      </c>
+      <c r="S505" t="s">
+        <v>43</v>
+      </c>
+      <c r="T505">
+        <v>754</v>
+      </c>
+      <c r="U505">
+        <v>0</v>
+      </c>
+      <c r="V505">
+        <v>0</v>
+      </c>
+      <c r="W505">
+        <v>0</v>
+      </c>
+      <c r="X505">
+        <v>28.5</v>
+      </c>
+      <c r="Y505">
+        <v>-14.33333</v>
+      </c>
+    </row>
+    <row r="506" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A506" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B506" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C506" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D506" t="s">
+        <v>48</v>
+      </c>
+      <c r="E506">
+        <v>2</v>
+      </c>
+      <c r="F506" t="s">
+        <v>49</v>
+      </c>
+      <c r="G506">
+        <v>202</v>
+      </c>
+      <c r="H506" t="s">
+        <v>107</v>
+      </c>
+      <c r="I506">
+        <v>14</v>
+      </c>
+      <c r="J506">
+        <v>716</v>
+      </c>
+      <c r="K506">
+        <v>0</v>
+      </c>
+      <c r="L506">
+        <v>1</v>
+      </c>
+      <c r="M506">
+        <v>0</v>
+      </c>
+      <c r="N506" t="s">
+        <v>31</v>
+      </c>
+      <c r="O506" t="s">
+        <v>51</v>
+      </c>
+      <c r="P506" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q506" t="s">
+        <v>49</v>
+      </c>
+      <c r="R506" t="s">
         <v>241</v>
       </c>
-      <c r="T505">
+      <c r="T506">
         <v>698</v>
       </c>
-      <c r="U505">
-        <v>0</v>
-      </c>
-      <c r="V505">
-        <v>0</v>
-      </c>
-      <c r="W505">
-        <v>0</v>
-      </c>
-      <c r="X505">
+      <c r="U506">
+        <v>0</v>
+      </c>
+      <c r="V506">
+        <v>0</v>
+      </c>
+      <c r="W506">
+        <v>0</v>
+      </c>
+      <c r="X506">
         <v>30.73189</v>
       </c>
-      <c r="Y505">
+      <c r="Y506">
         <v>-20.129123</v>
       </c>
     </row>
-    <row r="506" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="C506" t="s">
+    <row r="507" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="C507" t="s">
         <v>1022</v>
       </c>
-      <c r="D506" t="s">
+      <c r="D507" t="s">
         <v>61</v>
       </c>
-      <c r="E506">
+      <c r="E507">
         <v>150</v>
       </c>
-      <c r="F506" t="s">
+      <c r="F507" t="s">
         <v>62</v>
       </c>
-      <c r="G506">
+      <c r="G507">
         <v>154</v>
       </c>
-      <c r="H506" t="s">
+      <c r="H507" t="s">
         <v>379</v>
       </c>
-      <c r="I506">
+      <c r="I507">
         <v>830</v>
       </c>
-      <c r="J506">
+      <c r="J507">
         <v>680</v>
       </c>
-      <c r="K506">
-        <v>0</v>
-      </c>
-      <c r="L506">
-        <v>0</v>
-      </c>
-      <c r="M506">
-        <v>0</v>
-      </c>
-      <c r="N506" t="s">
+      <c r="K507">
+        <v>0</v>
+      </c>
+      <c r="L507">
+        <v>0</v>
+      </c>
+      <c r="M507">
+        <v>0</v>
+      </c>
+      <c r="N507" t="s">
         <v>63</v>
       </c>
-      <c r="V506">
-        <v>0</v>
-      </c>
-      <c r="W506">
+      <c r="V507">
+        <v>0</v>
+      </c>
+      <c r="W507">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y506">
-    <sortCondition ref="A2:A506"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y507">
+    <sortCondition ref="A2:A507"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>